<commit_message>
DC Motor Simulink Model
</commit_message>
<xml_diff>
--- a/Measurements/2018_10_07/motors.xlsx
+++ b/Measurements/2018_10_07/motors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\MSc\Final-Project\Measurements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\MSc\Final-Project\Measurements\2018_10_07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330CAEFD-2229-475A-A25B-235787E5D727}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B61E167-F2C9-4D8D-AE10-ABA349B8B2D8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="4875" xr2:uid="{631B157B-83C5-45A7-BE29-F12BE335A9BE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="4872" xr2:uid="{631B157B-83C5-45A7-BE29-F12BE335A9BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>T</t>
   </si>
@@ -47,19 +47,7 @@
     <t>I [A]</t>
   </si>
   <si>
-    <t>P [kgcm*rpm]</t>
-  </si>
-  <si>
     <t>w [rad/s]</t>
-  </si>
-  <si>
-    <t>T[N]</t>
-  </si>
-  <si>
-    <t>P[W]</t>
-  </si>
-  <si>
-    <t>K</t>
   </si>
   <si>
     <t>=</t>
@@ -72,6 +60,15 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>T[Nm]</t>
+  </si>
+  <si>
+    <t>Ri+Ldi/dt+Kw=U</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -271,7 +268,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Munka1!$G$4:$G$7</c:f>
+              <c:f>Munka1!$F$4:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -600,21 +597,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Munka1!$I$4:$I$7</c:f>
+              <c:f>Munka1!#REF!</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.2325515177583954</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.7326319111879123</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.9391369293143539</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -720,7 +708,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -980,7 +968,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Munka1!$H$3:$H$6</c:f>
+              <c:f>Munka1!$G$3:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1291,18 +1279,12 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Munka1!$K$4:$K$6</c:f>
+              <c:f>Munka1!$H$4:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>9.8170338729580316E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.9732080316477858E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.20029006846998693</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3730,13 +3712,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>192405</xdr:colOff>
+      <xdr:colOff>217755</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>11722</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -3765,16 +3747,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>596265</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>62865</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>306559</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>68725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>363854</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>189767</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>108731</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3803,16 +3785,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>519625</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>81915</xdr:rowOff>
+      <xdr:rowOff>122946</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>250141</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>119136</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3845,7 +3827,7 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>156210</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>26669</xdr:rowOff>
@@ -4173,28 +4155,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2660F20B-FEF9-46CB-8BFF-E5BD5B57FD16}">
-  <dimension ref="A2:Q7"/>
+  <dimension ref="A2:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="8" width="6.85546875" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" customWidth="1"/>
+    <col min="6" max="7" width="6.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -4211,25 +4191,22 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -4246,26 +4223,16 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="F3" s="1">
         <f>C3*0.0980665</f>
         <v>-0.10542148749999999</v>
       </c>
-      <c r="H3" s="1">
-        <f>G3+0.11</f>
+      <c r="G3" s="1">
+        <f>F3+0.11</f>
         <v>4.5785125000000065E-3</v>
       </c>
-      <c r="I3" s="4">
-        <f>F3*H3</f>
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>0.15</v>
       </c>
@@ -4278,45 +4245,40 @@
       <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
-        <f>C4*B4</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="E4" s="4">
         <f>2*PI()*B4/60</f>
         <v>11.205013797803595</v>
       </c>
-      <c r="G4" s="4">
+      <c r="F4" s="4">
         <f>C4*0.0980665</f>
         <v>0</v>
       </c>
-      <c r="H4" s="4">
-        <f t="shared" ref="H4:H7" si="0">G4+0.11</f>
+      <c r="G4" s="4">
+        <f t="shared" ref="G4:G7" si="0">F4+0.11</f>
         <v>0.11</v>
       </c>
-      <c r="I4" s="4">
-        <f>F4*H4</f>
-        <v>1.2325515177583954</v>
-      </c>
-      <c r="J4" s="4">
-        <f>H4/A4</f>
-        <v>0.73333333333333339</v>
-      </c>
-      <c r="K4" s="5">
-        <f>ABS(-H4)/F4</f>
+      <c r="H4" s="5">
+        <f>ABS(-G4)/E4</f>
         <v>9.8170338729580316E-3</v>
       </c>
-      <c r="O4" t="s">
+      <c r="I4">
+        <v>0.91479999999999995</v>
+      </c>
+      <c r="J4">
+        <f>(12-0.9148*107/60*2*PI())/0.15</f>
+        <v>11.664355851795149</v>
+      </c>
+      <c r="L4" t="s">
         <v>0</v>
       </c>
-      <c r="P4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>11</v>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>0.6</v>
       </c>
@@ -4329,39 +4291,24 @@
       <c r="D5" s="3">
         <v>3.8</v>
       </c>
-      <c r="E5" s="3">
-        <f>C5*B5</f>
-        <v>365.5</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="E5" s="4">
         <f>2*PI()*B5/60</f>
         <v>8.9011791851710811</v>
       </c>
-      <c r="G5" s="4">
+      <c r="F5" s="4">
         <f>C5*0.0980665</f>
         <v>0.42168594999999998</v>
       </c>
-      <c r="H5" s="4">
+      <c r="G5" s="4">
         <f t="shared" si="0"/>
         <v>0.53168594999999996</v>
       </c>
-      <c r="I5" s="4">
-        <f t="shared" ref="I5:I7" si="1">F5*H5</f>
-        <v>4.7326319111879123</v>
-      </c>
-      <c r="J5" s="4">
-        <f t="shared" ref="J5:J7" si="2">H5/A5</f>
-        <v>0.88614324999999994</v>
-      </c>
-      <c r="K5" s="5">
-        <f t="shared" ref="K5:K6" si="3">ABS(-H5)/F5</f>
-        <v>5.9732080316477858E-2</v>
-      </c>
-      <c r="P5" t="s">
-        <v>12</v>
+      <c r="H5" s="5"/>
+      <c r="M5" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>1.2</v>
       </c>
@@ -4374,36 +4321,21 @@
       <c r="D6" s="3">
         <v>6</v>
       </c>
-      <c r="E6" s="3">
-        <f>C6*B6</f>
-        <v>520</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="E6" s="4">
         <f>2*PI()*B6/60</f>
         <v>5.4454272662223087</v>
       </c>
-      <c r="G6" s="4">
+      <c r="F6" s="4">
         <f>C6*0.0980665</f>
         <v>0.98066500000000001</v>
       </c>
-      <c r="H6" s="4">
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>1.090665</v>
       </c>
-      <c r="I6" s="4">
-        <f t="shared" si="1"/>
-        <v>5.9391369293143539</v>
-      </c>
-      <c r="J6" s="4">
-        <f t="shared" si="2"/>
-        <v>0.90888750000000007</v>
-      </c>
-      <c r="K6" s="5">
-        <f t="shared" si="3"/>
-        <v>0.20029006846998693</v>
-      </c>
+      <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3.4</v>
       </c>
@@ -4416,31 +4348,19 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7">
-        <f>C7*B7</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="E7" s="1">
         <f>2*PI()*B7/60</f>
         <v>0</v>
       </c>
-      <c r="G7" s="1">
+      <c r="F7" s="1">
         <f>C7*0.0980665</f>
         <v>1.96133</v>
       </c>
-      <c r="H7" s="1">
+      <c r="G7" s="1">
         <f t="shared" si="0"/>
         <v>2.0713300000000001</v>
       </c>
-      <c r="I7" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="2"/>
-        <v>0.60921470588235294</v>
-      </c>
-      <c r="K7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>